<commit_message>
solve some issue with the printing of the results
</commit_message>
<xml_diff>
--- a/Instances/G0041111_NonStationary_b2_fe25_en_rk50_ll0_l20_HTrue6_c2.xlsx
+++ b/Instances/G0041111_NonStationary_b2_fe25_en_rk50_ll0_l20_HTrue6_c2.xlsx
@@ -518,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1854,7 +1854,7 @@
         <v>70</v>
       </c>
       <c r="H2" t="n">
-        <v>10.21142578125</v>
+        <v>10.20442708333333</v>
       </c>
       <c r="I2" t="n">
         <v>80</v>
@@ -1886,7 +1886,7 @@
         <v>30</v>
       </c>
       <c r="H3" t="n">
-        <v>4.463341346153846</v>
+        <v>3.789930555555555</v>
       </c>
       <c r="I3" t="n">
         <v>140</v>
@@ -1918,7 +1918,7 @@
         <v>50</v>
       </c>
       <c r="H4" t="n">
-        <v>5.351956881009615</v>
+        <v>7.555555555555555</v>
       </c>
       <c r="I4" t="n">
         <v>120</v>
@@ -1950,7 +1950,7 @@
         <v>100</v>
       </c>
       <c r="H5" t="n">
-        <v>16.40916090745192</v>
+        <v>9.999131944444445</v>
       </c>
       <c r="I5" t="n">
         <v>60</v>
@@ -2162,7 +2162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2312,13 +2312,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" t="n">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
         <v>84</v>
@@ -2347,16 +2347,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C6" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D6" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E6" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2382,16 +2382,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C7" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E7" t="n">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2417,16 +2417,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C8" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E8" t="n">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2452,16 +2452,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="C9" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="E9" t="n">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2487,16 +2487,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C10" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="E10" t="n">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2514,146 +2514,6 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>70</v>
-      </c>
-      <c r="C11" t="n">
-        <v>13</v>
-      </c>
-      <c r="D11" t="n">
-        <v>29</v>
-      </c>
-      <c r="E11" t="n">
-        <v>83</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>27</v>
-      </c>
-      <c r="C12" t="n">
-        <v>21</v>
-      </c>
-      <c r="D12" t="n">
-        <v>48</v>
-      </c>
-      <c r="E12" t="n">
-        <v>186</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>88</v>
-      </c>
-      <c r="C13" t="n">
-        <v>14</v>
-      </c>
-      <c r="D13" t="n">
-        <v>54</v>
-      </c>
-      <c r="E13" t="n">
-        <v>138</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>74</v>
-      </c>
-      <c r="C14" t="n">
-        <v>24</v>
-      </c>
-      <c r="D14" t="n">
-        <v>23</v>
-      </c>
-      <c r="E14" t="n">
-        <v>97</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2668,7 +2528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2818,13 +2678,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7.125</v>
+        <v>10.75</v>
       </c>
       <c r="C5" t="n">
-        <v>4.75</v>
+        <v>4.375</v>
       </c>
       <c r="D5" t="n">
-        <v>8.5</v>
+        <v>1.5</v>
       </c>
       <c r="E5" t="n">
         <v>10.5</v>
@@ -2853,16 +2713,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>13.125</v>
+        <v>13.5</v>
       </c>
       <c r="C6" t="n">
-        <v>8.0625</v>
+        <v>6.1875</v>
       </c>
       <c r="D6" t="n">
-        <v>13.3125</v>
+        <v>15.375</v>
       </c>
       <c r="E6" t="n">
-        <v>21.75</v>
+        <v>21.5625</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -2888,16 +2748,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>15.09375</v>
+        <v>19.6875</v>
       </c>
       <c r="C7" t="n">
-        <v>6.125</v>
+        <v>5.03125</v>
       </c>
       <c r="D7" t="n">
-        <v>1.09375</v>
+        <v>6.34375</v>
       </c>
       <c r="E7" t="n">
-        <v>16.40625</v>
+        <v>2.625</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2923,16 +2783,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>13.125</v>
+        <v>9.140625</v>
       </c>
       <c r="C8" t="n">
-        <v>8.671875</v>
+        <v>6.796875</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>10.3125</v>
       </c>
       <c r="E8" t="n">
-        <v>11.015625</v>
+        <v>13.359375</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -2958,16 +2818,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>11.140625</v>
+        <v>22.765625</v>
       </c>
       <c r="C9" t="n">
-        <v>4.84375</v>
+        <v>5.8125</v>
       </c>
       <c r="D9" t="n">
-        <v>3.875</v>
+        <v>14.2890625</v>
       </c>
       <c r="E9" t="n">
-        <v>13.5625</v>
+        <v>23.734375</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2993,16 +2853,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8.61328125</v>
+        <v>15.99609375</v>
       </c>
       <c r="C10" t="n">
-        <v>7.62890625</v>
+        <v>5.90625</v>
       </c>
       <c r="D10" t="n">
-        <v>4.4296875</v>
+        <v>20.1796875</v>
       </c>
       <c r="E10" t="n">
-        <v>14.51953125</v>
+        <v>18.2109375</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -3020,146 +2880,6 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>17.36328125</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3.224609375</v>
-      </c>
-      <c r="D11" t="n">
-        <v>7.193359375</v>
-      </c>
-      <c r="E11" t="n">
-        <v>20.587890625</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>6.7236328125</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5.2294921875</v>
-      </c>
-      <c r="D12" t="n">
-        <v>11.953125</v>
-      </c>
-      <c r="E12" t="n">
-        <v>46.318359375</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>21.95703125</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.4931640625</v>
-      </c>
-      <c r="D13" t="n">
-        <v>13.4736328125</v>
-      </c>
-      <c r="E13" t="n">
-        <v>34.4326171875</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>18.48193359375</v>
-      </c>
-      <c r="C14" t="n">
-        <v>5.994140625</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5.744384765625</v>
-      </c>
-      <c r="E14" t="n">
-        <v>24.226318359375</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3192,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>432</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3200,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>554</v>
+        <v>618</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3208,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>850</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>